<commit_message>
work on WS2812B program
</commit_message>
<xml_diff>
--- a/WS2812B_AddressableLED_TM4C123/calc.xlsx
+++ b/WS2812B_AddressableLED_TM4C123/calc.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexandru.gaal\Documents\GitHub\Embedded_Programs\WS2812B_AddressableLED_TM4C123\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="150" windowWidth="20055" windowHeight="7935"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -90,8 +95,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,6 +334,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -427,7 +440,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -459,9 +472,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -493,6 +507,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -668,14 +683,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:V25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="Q16" sqref="Q16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
@@ -687,7 +702,7 @@
     <col min="14" max="21" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="17" t="s">
         <v>17</v>
       </c>
@@ -714,7 +729,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="15.75" thickBot="1">
+    <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>18</v>
       </c>
@@ -744,7 +759,7 @@
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
     </row>
-    <row r="3" spans="1:22" ht="15.75" thickBot="1">
+    <row r="3" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="17"/>
       <c r="B3" s="17">
         <f>B1+B2</f>
@@ -790,7 +805,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:22">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B4" s="17">
         <f>B3+0.3</f>
         <v>1.55</v>
@@ -814,7 +829,7 @@
       <c r="T4" s="30"/>
       <c r="U4" s="31"/>
     </row>
-    <row r="5" spans="1:22" ht="15.75" thickBot="1">
+    <row r="5" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="15" t="s">
         <v>11</v>
       </c>
@@ -858,7 +873,7 @@
       <c r="T5" s="24"/>
       <c r="U5" s="24"/>
     </row>
-    <row r="6" spans="1:22" ht="15.75" thickBot="1">
+    <row r="6" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E6" s="28"/>
       <c r="K6" s="2">
         <f>K5*1000000</f>
@@ -896,7 +911,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>10</v>
       </c>
@@ -943,7 +958,7 @@
       <c r="U7" s="31"/>
       <c r="V7" s="27"/>
     </row>
-    <row r="8" spans="1:22">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B8" s="15">
         <f>B7*1000000</f>
         <v>0.15625</v>
@@ -952,13 +967,13 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="G9">
         <f>G7*6</f>
         <v>38.400000000000006</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="15.75" thickBot="1">
+    <row r="10" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J10" s="1" t="s">
         <v>12</v>
       </c>
@@ -969,7 +984,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:22">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="s">
         <v>1</v>
       </c>
@@ -995,7 +1010,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:22">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B12" s="9" t="s">
         <v>2</v>
       </c>
@@ -1021,7 +1036,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:22">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B13" s="9"/>
       <c r="C13" s="10"/>
       <c r="D13" s="11"/>
@@ -1033,7 +1048,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:22">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
         <v>3</v>
       </c>
@@ -1056,7 +1071,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="15.75" thickBot="1">
+    <row r="15" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="12" t="s">
         <v>4</v>
       </c>
@@ -1079,7 +1094,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:22">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="K16" s="2">
         <f>K15*8</f>
         <v>1.2</v>
@@ -1088,7 +1103,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="10:12">
+    <row r="17" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="Q17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J19" s="1" t="s">
         <v>12</v>
       </c>
@@ -1098,8 +1118,11 @@
       <c r="L19" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="10:12">
+      <c r="O19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="10:17" x14ac:dyDescent="0.25">
       <c r="J20" s="1" t="s">
         <v>13</v>
       </c>
@@ -1107,8 +1130,12 @@
         <v>16</v>
       </c>
       <c r="L20" s="3"/>
-    </row>
-    <row r="21" spans="10:12">
+      <c r="O20">
+        <f>MOD(O19+1,$Q$17)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="10:17" x14ac:dyDescent="0.25">
       <c r="K21" s="2">
         <f>K19/K20</f>
         <v>5</v>
@@ -1116,8 +1143,12 @@
       <c r="L21" s="3" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="10:12">
+      <c r="O21">
+        <f t="shared" ref="O21:O38" si="0">MOD(O20+1,$Q$17)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="10:17" x14ac:dyDescent="0.25">
       <c r="K22" s="2">
         <f>K21*1000000</f>
         <v>5000000</v>
@@ -1125,8 +1156,12 @@
       <c r="L22" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="23" spans="10:12">
+      <c r="O22">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="10:17" x14ac:dyDescent="0.25">
       <c r="K23" s="2">
         <f>1/K22</f>
         <v>1.9999999999999999E-7</v>
@@ -1134,8 +1169,12 @@
       <c r="L23" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="10:12">
+      <c r="O23">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="10:17" x14ac:dyDescent="0.25">
       <c r="K24" s="2">
         <f>K23*1000000</f>
         <v>0.19999999999999998</v>
@@ -1143,14 +1182,100 @@
       <c r="L24" s="3" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="25" spans="10:12">
+      <c r="O24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="10:17" x14ac:dyDescent="0.25">
       <c r="K25" s="2">
         <f>K24*8</f>
         <v>1.5999999999999999</v>
       </c>
       <c r="L25" s="3" t="s">
         <v>16</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="O26">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="O27">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="O28">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="O29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="O30">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="O31">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="10:17" x14ac:dyDescent="0.25">
+      <c r="O32">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O33">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O36">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O37">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="15:15" x14ac:dyDescent="0.25">
+      <c r="O38">
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -1165,24 +1290,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>